<commit_message>
Ghant chard is updated.
</commit_message>
<xml_diff>
--- a/Course Materials/Gantt Chard_Production.xlsx
+++ b/Course Materials/Gantt Chard_Production.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>PERIODS</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Manufacturing of Tilt Mechanism</t>
   </si>
   <si>
-    <t>Assembly of the Aircraft Body</t>
-  </si>
-  <si>
     <t>Software Configuration and Maiden Flight</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>Production of a vertical take-off and landing aircraft process</t>
+  </si>
+  <si>
+    <t>Assembly of the Aircraft</t>
   </si>
 </sst>
 </file>
@@ -1259,8 +1259,8 @@
   </sheetPr>
   <dimension ref="A2:AB30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="61" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AP9" sqref="AP9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1308,7 +1308,7 @@
     <row r="3" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="6" t="s">
@@ -1458,14 +1458,14 @@
       <c r="D6" s="30">
         <v>2</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>28</v>
+      <c r="E6" s="30">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30">
+        <v>2</v>
       </c>
       <c r="G6" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="9"/>
@@ -1490,23 +1490,23 @@
     </row>
     <row r="7" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
-      <c r="B7" s="34" t="s">
-        <v>15</v>
+      <c r="B7" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="27">
         <v>2</v>
       </c>
       <c r="D7" s="31">
-        <v>3</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="E7" s="31">
+        <v>2</v>
+      </c>
+      <c r="F7" s="31">
+        <v>1</v>
       </c>
       <c r="G7" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="13"/>
@@ -1531,23 +1531,23 @@
     </row>
     <row r="8" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
-      <c r="B8" s="34" t="s">
-        <v>17</v>
+      <c r="B8" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="27">
         <v>2</v>
       </c>
       <c r="D8" s="31">
-        <v>3</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="E8" s="31">
+        <v>2</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
       </c>
       <c r="G8" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="13"/>
@@ -1566,26 +1566,25 @@
       <c r="V8" s="14"/>
       <c r="W8"/>
       <c r="X8"/>
-      <c r="Y8"/>
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
     <row r="9" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
-      <c r="B9" s="35" t="s">
-        <v>16</v>
+      <c r="B9" s="34" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="17">
         <v>0</v>
@@ -1607,26 +1606,25 @@
       <c r="V9" s="14"/>
       <c r="W9"/>
       <c r="X9"/>
-      <c r="Y9"/>
       <c r="Z9"/>
       <c r="AA9"/>
     </row>
     <row r="10" spans="1:28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
-      <c r="B10" s="36" t="s">
-        <v>24</v>
+      <c r="B10" s="34" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="17">
         <v>0</v>
@@ -1664,10 +1662,10 @@
         <v>3</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="17">
         <v>0</v>
@@ -1699,16 +1697,16 @@
         <v>19</v>
       </c>
       <c r="C12" s="27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="17">
         <v>0</v>
@@ -1746,10 +1744,10 @@
         <v>3</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="17">
         <v>0</v>
@@ -1787,10 +1785,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="17">
         <v>0</v>
@@ -1828,10 +1826,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="17">
         <v>0</v>
@@ -1869,10 +1867,10 @@
         <v>2</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="17">
         <v>0</v>
@@ -1901,7 +1899,7 @@
     <row r="17" spans="1:27" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="34" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C17" s="29">
         <v>12</v>
@@ -1910,10 +1908,10 @@
         <v>2</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="17">
         <v>0</v>
@@ -1951,10 +1949,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G18" s="17">
         <v>0</v>
@@ -1982,7 +1980,7 @@
     </row>
     <row r="19" spans="1:27" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="27">
         <v>13</v>
@@ -1991,10 +1989,10 @@
         <v>3</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G19" s="17">
         <v>0</v>
@@ -2082,7 +2080,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="16">
+  <dataValidations count="16">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A2"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="G3">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>

</xml_diff>

<commit_message>
Gantt Chard has been updated.
</commit_message>
<xml_diff>
--- a/Course Materials/Gantt Chard_Production.xlsx
+++ b/Course Materials/Gantt Chard_Production.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>PERIODS</t>
   </si>
@@ -1259,8 +1259,8 @@
   </sheetPr>
   <dimension ref="A2:AB30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="6" t="s">
@@ -1580,14 +1580,14 @@
       <c r="D9" s="31">
         <v>3</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>27</v>
+      <c r="E9" s="31">
+        <v>3</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="17">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="13"/>

</xml_diff>